<commit_message>
modified grad_a calc method, added consideration of ATO余量
</commit_message>
<xml_diff>
--- a/线路条件数据.xlsx
+++ b/线路条件数据.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24760" windowHeight="12240" activeTab="3"/>
+    <workbookView windowWidth="16500" windowHeight="10200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="station" sheetId="1" r:id="rId1"/>
@@ -296,7 +296,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,13 +307,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -772,148 +765,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2760,7 +2753,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -3606,12 +3599,15 @@
   <sheetPr/>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
   <cols>
+    <col min="8" max="8" width="24.6964285714286" customWidth="1"/>
+    <col min="9" max="9" width="16.2232142857143" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="20.6607142857143" customWidth="1"/>
   </cols>

</xml_diff>